<commit_message>
Resolved error 1000 in pre-enumeration survey
</commit_message>
<xml_diff>
--- a/Community/Pre-Enumeration_Survey.xlsx
+++ b/Community/Pre-Enumeration_Survey.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mitchell\Documents\Survey123 Samples and Templates\Community Surveys\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\applications\Survey123templates\Survey123Community\Community\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13180" tabRatio="203"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6470" tabRatio="203"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -18,11 +18,16 @@
     <sheet name="types" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1224" uniqueCount="1047">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1226" uniqueCount="1049">
   <si>
     <t>type</t>
   </si>
@@ -3163,6 +3168,12 @@
   </si>
   <si>
     <t>XMLVALIDATE</t>
+  </si>
+  <si>
+    <t>bind::type</t>
+  </si>
+  <si>
+    <t>int</t>
   </si>
 </sst>
 </file>
@@ -3582,9 +3593,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:X236" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="A1:X236"/>
-  <tableColumns count="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:Y236" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="A1:Y236"/>
+  <tableColumns count="25">
     <tableColumn id="1" name="type"/>
     <tableColumn id="2" name="name"/>
     <tableColumn id="3" name="label" dataDxfId="4"/>
@@ -3609,6 +3620,7 @@
     <tableColumn id="18" name="bind::esri:fieldLength"/>
     <tableColumn id="23" name="bind::esri:fieldAlias"/>
     <tableColumn id="22" name="body::esri:inputMask"/>
+    <tableColumn id="25" name="bind::type"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3924,7 +3936,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -3966,7 +3978,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -3989,13 +4001,13 @@
   <dimension ref="A1:AF29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <pane xSplit="3" topLeftCell="V1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.453125" defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="19.54296875" customWidth="1"/>
+    <col min="1" max="2" width="19.453125" customWidth="1"/>
     <col min="3" max="3" width="49" style="6" customWidth="1"/>
     <col min="4" max="4" width="62.81640625" style="1" customWidth="1"/>
     <col min="6" max="6" width="24.453125" style="1"/>
@@ -4074,7 +4086,9 @@
       <c r="X1" s="24" t="s">
         <v>264</v>
       </c>
-      <c r="Y1" s="2"/>
+      <c r="Y1" s="12" t="s">
+        <v>1047</v>
+      </c>
       <c r="Z1" s="2"/>
       <c r="AA1" s="2"/>
       <c r="AB1" s="2"/>
@@ -4477,7 +4491,7 @@
       <c r="Q16" s="27"/>
       <c r="R16" s="27"/>
     </row>
-    <row r="17" spans="1:22" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="27" t="s">
         <v>314</v>
       </c>
@@ -4507,7 +4521,7 @@
       <c r="Q17" s="27"/>
       <c r="R17" s="27"/>
     </row>
-    <row r="18" spans="1:22" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="27" t="s">
         <v>318</v>
       </c>
@@ -4533,7 +4547,7 @@
       <c r="Q18" s="27"/>
       <c r="R18" s="27"/>
     </row>
-    <row r="19" spans="1:22" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="27" t="s">
         <v>322</v>
       </c>
@@ -4559,7 +4573,7 @@
       <c r="Q19" s="27"/>
       <c r="R19" s="27"/>
     </row>
-    <row r="20" spans="1:22" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="27" t="s">
         <v>35</v>
       </c>
@@ -4585,7 +4599,7 @@
       <c r="Q20" s="27"/>
       <c r="R20" s="27"/>
     </row>
-    <row r="21" spans="1:22" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="27" t="s">
         <v>24</v>
       </c>
@@ -4613,7 +4627,7 @@
       <c r="Q21" s="27"/>
       <c r="R21" s="27"/>
     </row>
-    <row r="22" spans="1:22" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="27" t="s">
         <v>24</v>
       </c>
@@ -4641,7 +4655,7 @@
       <c r="Q22" s="27"/>
       <c r="R22" s="27"/>
     </row>
-    <row r="23" spans="1:22" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="27" t="s">
         <v>122</v>
       </c>
@@ -4670,8 +4684,11 @@
       <c r="V23" s="27">
         <v>3</v>
       </c>
-    </row>
-    <row r="24" spans="1:22" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Y23" t="s">
+        <v>1048</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="27" t="s">
         <v>336</v>
       </c>
@@ -4701,7 +4718,7 @@
       <c r="Q24" s="27"/>
       <c r="R24" s="27"/>
     </row>
-    <row r="25" spans="1:22" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="27" t="s">
         <v>36</v>
       </c>
@@ -4721,7 +4738,7 @@
       <c r="Q25" s="27"/>
       <c r="R25" s="27"/>
     </row>
-    <row r="26" spans="1:22" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="27" t="s">
         <v>10</v>
       </c>
@@ -4745,7 +4762,7 @@
       <c r="Q26" s="27"/>
       <c r="R26" s="27"/>
     </row>
-    <row r="27" spans="1:22" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="27" t="s">
         <v>221</v>
       </c>
@@ -4767,7 +4784,7 @@
       <c r="Q27" s="27"/>
       <c r="R27" s="27"/>
     </row>
-    <row r="28" spans="1:22" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="27" t="s">
         <v>227</v>
       </c>
@@ -4791,7 +4808,7 @@
       <c r="Q28" s="27"/>
       <c r="R28" s="27"/>
     </row>
-    <row r="29" spans="1:22" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="27" t="s">
         <v>228</v>
       </c>
@@ -4902,11 +4919,11 @@
   <dimension ref="A1:E60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.54296875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="13.453125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.453125" customWidth="1"/>
     <col min="2" max="2" width="17.453125" customWidth="1"/>
@@ -5517,7 +5534,7 @@
     <col min="1" max="1" width="22.81640625" customWidth="1"/>
     <col min="2" max="2" width="16.453125" customWidth="1"/>
     <col min="3" max="3" width="14.81640625" customWidth="1"/>
-    <col min="4" max="4" width="24.54296875" customWidth="1"/>
+    <col min="4" max="4" width="24.453125" customWidth="1"/>
     <col min="5" max="5" width="18.453125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5563,14 +5580,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L795"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection sqref="A1:L795"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.453125" customWidth="1"/>
-    <col min="2" max="2" width="74.54296875" customWidth="1"/>
+    <col min="2" max="2" width="74.453125" customWidth="1"/>
     <col min="3" max="3" width="52.81640625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -17826,10 +17841,5 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>